<commit_message>
Update statistics  about job
</commit_message>
<xml_diff>
--- a/EBooks/中队就业信息统计-软三信息.xlsx
+++ b/EBooks/中队就业信息统计-软三信息.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>学院（系）</t>
   </si>
@@ -328,7 +328,10 @@
     <t xml:space="preserve">6（张伟-天津理工大学， 范玉龙-大连海事大学，王林辉-大连海事大学， 辛晓宇-大连海事大学， 马晓雅-北京理工大学， 陈艺燕-福州大学） </t>
   </si>
   <si>
-    <t>7（准备公务员，准备今年考研，另有打算）</t>
+    <t>7（马玉娟，姚丹，卢任强，田广予，王淙澜， 侯一凡，郭新乐）（准备公务员，准备今年考研，另有打算）</t>
+  </si>
+  <si>
+    <t>1（王润飞）</t>
   </si>
 </sst>
 </file>
@@ -1058,7 +1061,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1356,8 +1359,8 @@
         <v>34</v>
       </c>
       <c r="N11" s="23"/>
-      <c r="O11" s="4">
-        <v>1</v>
+      <c r="O11" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="P11" s="4">
         <v>14</v>

</xml_diff>